<commit_message>
fixes in 1 task
</commit_message>
<xml_diff>
--- a/Problems 1.xlsx
+++ b/Problems 1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="10848" windowHeight="9192"/>
+    <workbookView windowWidth="22368" windowHeight="9335"/>
   </bookViews>
   <sheets>
     <sheet name="Var2" sheetId="4" r:id="rId1"/>
@@ -2486,8 +2486,8 @@
   <sheetPr/>
   <dimension ref="A2:AJ423"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" topLeftCell="H287" workbookViewId="0">
-      <selection activeCell="N295" sqref="N295"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" topLeftCell="A345" workbookViewId="0">
+      <selection activeCell="P354" sqref="P354"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>

</xml_diff>